<commit_message>
tabla de aportes init
</commit_message>
<xml_diff>
--- a/data/miembros.xlsx
+++ b/data/miembros.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20386"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\2018001\OneDrive - Banco Central de la Republica Dominicana\Desktop\Proyectos\goat_app\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8feae05406065f8f/Desktop/proyectos_r/1-personales/goat/App/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C40AC0FF-3A7F-4E5D-AB99-CBECBAF74402}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="16" documentId="13_ncr:1_{C40AC0FF-3A7F-4E5D-AB99-CBECBAF74402}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E67B7AD4-998F-204A-9F3C-0EB4124676A5}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8940" xr2:uid="{E69FF370-BCB9-4155-8F01-725C61F4E151}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="23780" windowHeight="15000" xr2:uid="{E69FF370-BCB9-4155-8F01-725C61F4E151}"/>
   </bookViews>
   <sheets>
     <sheet name="Lista de miembros" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="58">
   <si>
     <t>Johan</t>
   </si>
@@ -78,9 +78,6 @@
     <t>Yandi</t>
   </si>
   <si>
-    <t>Amio de Kibelo</t>
-  </si>
-  <si>
     <t>Orlando</t>
   </si>
   <si>
@@ -120,9 +117,6 @@
     <t>Apodo</t>
   </si>
   <si>
-    <t>El Ribio</t>
-  </si>
-  <si>
     <t>Michael</t>
   </si>
   <si>
@@ -157,6 +151,54 @@
   </si>
   <si>
     <t>Julio</t>
+  </si>
+  <si>
+    <t>avatar_img</t>
+  </si>
+  <si>
+    <t>johan.jpg</t>
+  </si>
+  <si>
+    <t>alfredo.jpg</t>
+  </si>
+  <si>
+    <t>rayder.jpg</t>
+  </si>
+  <si>
+    <t>jeicol.jpg</t>
+  </si>
+  <si>
+    <t>yeyo.jpg</t>
+  </si>
+  <si>
+    <t>randy.jpg</t>
+  </si>
+  <si>
+    <t>punto.jpg</t>
+  </si>
+  <si>
+    <t>joel.jpg</t>
+  </si>
+  <si>
+    <t>cristopher.jpg</t>
+  </si>
+  <si>
+    <t>kukito.jpg</t>
+  </si>
+  <si>
+    <t>omauri.jpg</t>
+  </si>
+  <si>
+    <t>carlos.jpg</t>
+  </si>
+  <si>
+    <t>kawai.jpg</t>
+  </si>
+  <si>
+    <t>El Rubio</t>
+  </si>
+  <si>
+    <t>Amigo de Kibelo</t>
   </si>
 </sst>
 </file>
@@ -212,14 +254,14 @@
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -239,8 +281,12 @@
 </styleSheet>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2013 - 2022">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -528,7 +574,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -536,60 +582,66 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE220CC2-8725-42B3-AD79-7FD328EB1B49}">
-  <dimension ref="A1:C35"/>
+  <dimension ref="A1:D35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="4.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.28515625" customWidth="1"/>
+    <col min="1" max="1" width="4.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="C1" t="s">
         <v>29</v>
       </c>
-      <c r="C1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="4">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="4">
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C3" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="4">
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C4" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="4">
         <v>4</v>
       </c>
@@ -597,32 +649,38 @@
         <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="4">
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C6" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+      <c r="D6" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="4">
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C7" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+      <c r="D7" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="4">
         <v>7</v>
       </c>
@@ -630,34 +688,40 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="4">
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D9" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="4">
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D10" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="4">
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C11" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="4">
         <v>11</v>
       </c>
@@ -665,7 +729,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" s="4">
         <v>12</v>
       </c>
@@ -675,8 +739,11 @@
       <c r="C13" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D13" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" s="4">
         <v>13</v>
       </c>
@@ -684,15 +751,18 @@
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" s="4">
         <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D15" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" s="4">
         <v>15</v>
       </c>
@@ -700,18 +770,18 @@
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" s="4">
         <v>16</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C17" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="4">
         <v>17</v>
       </c>
@@ -719,7 +789,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" s="4">
         <v>18</v>
       </c>
@@ -727,7 +797,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" s="4">
         <v>19</v>
       </c>
@@ -735,15 +805,18 @@
         <v>12</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" s="4">
         <v>20</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D21" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" s="4">
         <v>21</v>
       </c>
@@ -751,7 +824,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" s="4">
         <v>22</v>
       </c>
@@ -759,7 +832,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" s="4">
         <v>23</v>
       </c>
@@ -767,92 +840,107 @@
         <v>16</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" s="4">
         <v>24</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" s="4">
         <v>25</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" s="4">
         <v>26</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+      <c r="D27" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" s="4">
         <v>27</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+      <c r="D28" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" s="4">
         <v>28</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" s="4">
         <v>29</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+      <c r="D30" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" s="4">
         <v>30</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" s="4">
         <v>31</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+      <c r="D32" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" s="4">
         <v>32</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" s="4">
         <v>33</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+      <c r="D34" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" s="4">
         <v>34</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>